<commit_message>
remove backups (which were updated)
</commit_message>
<xml_diff>
--- a/Log Activity.xlsx
+++ b/Log Activity.xlsx
@@ -549,6 +549,652 @@
       <c r="G2" s="6" t="n"/>
       <c r="H2" t="inlineStr">
         <is>
+          <t>ERROR: ('Connection aborted.', ConnectionResetError(10054, 'An existing connection was forcibly closed by the remote host', None, 10054, None))</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="n">
+        <v>120242152</v>
+      </c>
+      <c r="B3" s="4" t="inlineStr">
+        <is>
+          <t>elliTek</t>
+        </is>
+      </c>
+      <c r="C3" s="5" t="inlineStr">
+        <is>
+          <t>alan penticuff</t>
+        </is>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>120206934</v>
+      </c>
+      <c r="E3" s="6" t="inlineStr">
+        <is>
+          <t>weidmuller cross</t>
+        </is>
+      </c>
+      <c r="F3" s="5" t="inlineStr">
+        <is>
+          <t>20260105</t>
+        </is>
+      </c>
+      <c r="G3" s="6" t="n"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>ERROR: HTTPConnectionPool(host='localhost', port=58522): Max retries exceeded with url: /session/182bcb18ac3fbf462df686da6b43a0f5/element (Caused by NewConnectionError("HTTPConnection(host='localhost', port=58522): Failed to establish a new connection: [WinError 10061] No connection could be made because the target machine actively refused it"))</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="n">
+        <v>120032621</v>
+      </c>
+      <c r="B4" s="4" t="inlineStr">
+        <is>
+          <t>Control Systems Inc</t>
+        </is>
+      </c>
+      <c r="C4" s="5" t="inlineStr">
+        <is>
+          <t>James Mason</t>
+        </is>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>120032620</v>
+      </c>
+      <c r="E4" s="6" t="inlineStr">
+        <is>
+          <t>IIAT Visit</t>
+        </is>
+      </c>
+      <c r="F4" s="5" t="inlineStr">
+        <is>
+          <t>20251210</t>
+        </is>
+      </c>
+      <c r="G4" s="6" t="n"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>ERROR: HTTPConnectionPool(host='localhost', port=58522): Max retries exceeded with url: /session/182bcb18ac3fbf462df686da6b43a0f5/element (Caused by NewConnectionError("HTTPConnection(host='localhost', port=58522): Failed to establish a new connection: [WinError 10061] No connection could be made because the target machine actively refused it"))</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="n">
+        <v>120288152</v>
+      </c>
+      <c r="B5" s="4" t="inlineStr">
+        <is>
+          <t>Control Systems Inc.</t>
+        </is>
+      </c>
+      <c r="C5" s="5" t="inlineStr">
+        <is>
+          <t>Charlie Roberts</t>
+        </is>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>120032620</v>
+      </c>
+      <c r="E5" s="6" t="inlineStr">
+        <is>
+          <t>IIAT Visit</t>
+        </is>
+      </c>
+      <c r="F5" s="5" t="inlineStr">
+        <is>
+          <t>20251210</t>
+        </is>
+      </c>
+      <c r="G5" s="6" t="n"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>ERROR: HTTPConnectionPool(host='localhost', port=58522): Max retries exceeded with url: /session/182bcb18ac3fbf462df686da6b43a0f5/element (Caused by NewConnectionError("HTTPConnection(host='localhost', port=58522): Failed to establish a new connection: [WinError 10061] No connection could be made because the target machine actively refused it"))</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="n">
+        <v>120252514</v>
+      </c>
+      <c r="B6" s="4" t="inlineStr">
+        <is>
+          <t>Rotary Gate Systems</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="inlineStr">
+        <is>
+          <t>jim knoll</t>
+        </is>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>120252513</v>
+      </c>
+      <c r="E6" s="6" t="inlineStr">
+        <is>
+          <t>231 application</t>
+        </is>
+      </c>
+      <c r="F6" s="5" t="inlineStr">
+        <is>
+          <t>20251211</t>
+        </is>
+      </c>
+      <c r="G6" s="6" t="n"/>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>ERROR: HTTPConnectionPool(host='localhost', port=58522): Max retries exceeded with url: /session/182bcb18ac3fbf462df686da6b43a0f5/element (Caused by NewConnectionError("HTTPConnection(host='localhost', port=58522): Failed to establish a new connection: [WinError 10061] No connection could be made because the target machine actively refused it"))</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="n">
+        <v>120293516</v>
+      </c>
+      <c r="B7" s="4" t="inlineStr">
+        <is>
+          <t>Electric Power Research Institute, Inc EPRI</t>
+        </is>
+      </c>
+      <c r="C7" s="5" t="inlineStr">
+        <is>
+          <t>Ben Ealy</t>
+        </is>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>120214766</v>
+      </c>
+      <c r="E7" s="6" t="inlineStr">
+        <is>
+          <t>DER Controller Testing</t>
+        </is>
+      </c>
+      <c r="F7" s="5" t="inlineStr">
+        <is>
+          <t>20251105</t>
+        </is>
+      </c>
+      <c r="G7" s="6" t="n"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>ERROR: HTTPConnectionPool(host='localhost', port=58522): Max retries exceeded with url: /session/182bcb18ac3fbf462df686da6b43a0f5/element (Caused by NewConnectionError("HTTPConnection(host='localhost', port=58522): Failed to establish a new connection: [WinError 10061] No connection could be made because the target machine actively refused it"))</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="n">
+        <v>120293517</v>
+      </c>
+      <c r="B8" s="4" t="inlineStr">
+        <is>
+          <t>Electric Power Research Institute, Inc EPRI</t>
+        </is>
+      </c>
+      <c r="C8" s="5" t="inlineStr">
+        <is>
+          <t>Ibtissam Kharchouf</t>
+        </is>
+      </c>
+      <c r="D8" s="4" t="n">
+        <v>120214766</v>
+      </c>
+      <c r="E8" s="6" t="inlineStr">
+        <is>
+          <t>DER Controller Testing</t>
+        </is>
+      </c>
+      <c r="F8" s="5" t="inlineStr">
+        <is>
+          <t>20251105</t>
+        </is>
+      </c>
+      <c r="G8" s="6" t="n"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>ERROR: HTTPConnectionPool(host='localhost', port=58522): Max retries exceeded with url: /session/182bcb18ac3fbf462df686da6b43a0f5/element (Caused by NewConnectionError("HTTPConnection(host='localhost', port=58522): Failed to establish a new connection: [WinError 10061] No connection could be made because the target machine actively refused it"))</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="n">
+        <v>101035107</v>
+      </c>
+      <c r="B9" s="4" t="inlineStr">
+        <is>
+          <t>Mesa Associates, Inc.</t>
+        </is>
+      </c>
+      <c r="C9" s="5" t="inlineStr">
+        <is>
+          <t>Aneesh Davalbhakta</t>
+        </is>
+      </c>
+      <c r="D9" s="4" t="n">
+        <v>523553</v>
+      </c>
+      <c r="E9" s="6" t="inlineStr">
+        <is>
+          <t>Chris Dunlap meeting - scheduled Lunch n Learn</t>
+        </is>
+      </c>
+      <c r="F9" s="5" t="inlineStr">
+        <is>
+          <t>20251105</t>
+        </is>
+      </c>
+      <c r="G9" s="6" t="n"/>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>ERROR: HTTPConnectionPool(host='localhost', port=58522): Max retries exceeded with url: /session/182bcb18ac3fbf462df686da6b43a0f5/element (Caused by NewConnectionError("HTTPConnection(host='localhost', port=58522): Failed to establish a new connection: [WinError 10061] No connection could be made because the target machine actively refused it"))</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="n">
+        <v>101029218</v>
+      </c>
+      <c r="B10" s="4" t="inlineStr">
+        <is>
+          <t>AUTOMATION NTH</t>
+        </is>
+      </c>
+      <c r="C10" s="5" t="inlineStr">
+        <is>
+          <t>scott weeks</t>
+        </is>
+      </c>
+      <c r="D10" s="4" t="n">
+        <v>522371</v>
+      </c>
+      <c r="E10" s="6" t="inlineStr">
+        <is>
+          <t>Plan lunch n learn</t>
+        </is>
+      </c>
+      <c r="F10" s="5" t="inlineStr">
+        <is>
+          <t>20251106</t>
+        </is>
+      </c>
+      <c r="G10" s="6" t="n"/>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>ERROR: HTTPConnectionPool(host='localhost', port=58522): Max retries exceeded with url: /session/182bcb18ac3fbf462df686da6b43a0f5/element (Caused by NewConnectionError("HTTPConnection(host='localhost', port=58522): Failed to establish a new connection: [WinError 10061] No connection could be made because the target machine actively refused it"))</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="n">
+        <v>100949918</v>
+      </c>
+      <c r="B11" s="4" t="inlineStr">
+        <is>
+          <t>Automation Tool Company ATC</t>
+        </is>
+      </c>
+      <c r="C11" s="5" t="inlineStr">
+        <is>
+          <t>David Bailey</t>
+        </is>
+      </c>
+      <c r="D11" s="4" t="n">
+        <v>7438426</v>
+      </c>
+      <c r="E11" s="6" t="inlineStr">
+        <is>
+          <t>Trade Show</t>
+        </is>
+      </c>
+      <c r="F11" s="5" t="inlineStr">
+        <is>
+          <t>20251119</t>
+        </is>
+      </c>
+      <c r="G11" s="6" t="n"/>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>ERROR: HTTPConnectionPool(host='localhost', port=58522): Max retries exceeded with url: /session/182bcb18ac3fbf462df686da6b43a0f5/element (Caused by NewConnectionError("HTTPConnection(host='localhost', port=58522): Failed to establish a new connection: [WinError 10061] No connection could be made because the target machine actively refused it"))</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="n">
+        <v>100949916</v>
+      </c>
+      <c r="B12" s="4" t="inlineStr">
+        <is>
+          <t>Automation Tool Company ATC</t>
+        </is>
+      </c>
+      <c r="C12" s="5" t="inlineStr">
+        <is>
+          <t>Bobby Buck</t>
+        </is>
+      </c>
+      <c r="D12" s="4" t="n">
+        <v>7438426</v>
+      </c>
+      <c r="E12" s="6" t="inlineStr">
+        <is>
+          <t>Trade Show</t>
+        </is>
+      </c>
+      <c r="F12" s="5" t="inlineStr">
+        <is>
+          <t>20251119</t>
+        </is>
+      </c>
+      <c r="G12" s="6" t="n"/>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>ERROR: HTTPConnectionPool(host='localhost', port=58522): Max retries exceeded with url: /session/182bcb18ac3fbf462df686da6b43a0f5/element (Caused by NewConnectionError("HTTPConnection(host='localhost', port=58522): Failed to establish a new connection: [WinError 10061] No connection could be made because the target machine actively refused it"))</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="n">
+        <v>101092867</v>
+      </c>
+      <c r="B13" s="4" t="inlineStr">
+        <is>
+          <t>Automation Tool Company ATC</t>
+        </is>
+      </c>
+      <c r="C13" s="5" t="inlineStr">
+        <is>
+          <t>Andy Cannon</t>
+        </is>
+      </c>
+      <c r="D13" s="4" t="n">
+        <v>7438426</v>
+      </c>
+      <c r="E13" s="6" t="inlineStr">
+        <is>
+          <t>Trade Show</t>
+        </is>
+      </c>
+      <c r="F13" s="5" t="inlineStr">
+        <is>
+          <t>20251119</t>
+        </is>
+      </c>
+      <c r="G13" s="6" t="n"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>ERROR: HTTPConnectionPool(host='localhost', port=58522): Max retries exceeded with url: /session/182bcb18ac3fbf462df686da6b43a0f5/element (Caused by NewConnectionError("HTTPConnection(host='localhost', port=58522): Failed to establish a new connection: [WinError 10061] No connection could be made because the target machine actively refused it"))</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="4" t="n">
+        <v>101086797</v>
+      </c>
+      <c r="B14" s="4" t="inlineStr">
+        <is>
+          <t>Automation Tool Company ATC</t>
+        </is>
+      </c>
+      <c r="C14" s="5" t="inlineStr">
+        <is>
+          <t>Josh Forgey</t>
+        </is>
+      </c>
+      <c r="D14" s="4" t="n">
+        <v>7438426</v>
+      </c>
+      <c r="E14" s="6" t="inlineStr">
+        <is>
+          <t>Trade Show</t>
+        </is>
+      </c>
+      <c r="F14" s="5" t="inlineStr">
+        <is>
+          <t>20251119</t>
+        </is>
+      </c>
+      <c r="G14" s="6" t="n"/>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>ERROR: HTTPConnectionPool(host='localhost', port=58522): Max retries exceeded with url: /session/182bcb18ac3fbf462df686da6b43a0f5/element (Caused by NewConnectionError("HTTPConnection(host='localhost', port=58522): Failed to establish a new connection: [WinError 10061] No connection could be made because the target machine actively refused it"))</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="4" t="n">
+        <v>101140229</v>
+      </c>
+      <c r="B15" s="4" t="inlineStr">
+        <is>
+          <t>Automation Tool Company ATC</t>
+        </is>
+      </c>
+      <c r="C15" s="5" t="inlineStr">
+        <is>
+          <t>Nathan Gooch</t>
+        </is>
+      </c>
+      <c r="D15" s="4" t="n">
+        <v>7438426</v>
+      </c>
+      <c r="E15" s="6" t="inlineStr">
+        <is>
+          <t>Trade Show</t>
+        </is>
+      </c>
+      <c r="F15" s="5" t="inlineStr">
+        <is>
+          <t>20251119</t>
+        </is>
+      </c>
+      <c r="G15" s="6" t="n"/>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>ERROR: HTTPConnectionPool(host='localhost', port=58522): Max retries exceeded with url: /session/182bcb18ac3fbf462df686da6b43a0f5/element (Caused by NewConnectionError("HTTPConnection(host='localhost', port=58522): Failed to establish a new connection: [WinError 10061] No connection could be made because the target machine actively refused it"))</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="4" t="n">
+        <v>120053080</v>
+      </c>
+      <c r="B16" s="4" t="inlineStr">
+        <is>
+          <t>Automation Tool Company ATC</t>
+        </is>
+      </c>
+      <c r="C16" s="5" t="inlineStr">
+        <is>
+          <t>Raymond Kilpatrick</t>
+        </is>
+      </c>
+      <c r="D16" s="4" t="n">
+        <v>7438426</v>
+      </c>
+      <c r="E16" s="6" t="inlineStr">
+        <is>
+          <t>Trade Show</t>
+        </is>
+      </c>
+      <c r="F16" s="5" t="inlineStr">
+        <is>
+          <t>20251119</t>
+        </is>
+      </c>
+      <c r="G16" s="6" t="n"/>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>ERROR: HTTPConnectionPool(host='localhost', port=58522): Max retries exceeded with url: /session/182bcb18ac3fbf462df686da6b43a0f5/element (Caused by NewConnectionError("HTTPConnection(host='localhost', port=58522): Failed to establish a new connection: [WinError 10061] No connection could be made because the target machine actively refused it"))</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="4" t="n">
+        <v>101035097</v>
+      </c>
+      <c r="B17" s="4" t="inlineStr">
+        <is>
+          <t>Automation Tool Company ATC</t>
+        </is>
+      </c>
+      <c r="C17" s="5" t="inlineStr">
+        <is>
+          <t>Jake McGusland</t>
+        </is>
+      </c>
+      <c r="D17" s="4" t="n">
+        <v>7438426</v>
+      </c>
+      <c r="E17" s="6" t="inlineStr">
+        <is>
+          <t>Trade Show</t>
+        </is>
+      </c>
+      <c r="F17" s="5" t="inlineStr">
+        <is>
+          <t>20251119</t>
+        </is>
+      </c>
+      <c r="G17" s="6" t="n"/>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>ERROR: HTTPConnectionPool(host='localhost', port=58522): Max retries exceeded with url: /session/182bcb18ac3fbf462df686da6b43a0f5/element (Caused by NewConnectionError("HTTPConnection(host='localhost', port=58522): Failed to establish a new connection: [WinError 10061] No connection could be made because the target machine actively refused it"))</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="4" t="n">
+        <v>120051335</v>
+      </c>
+      <c r="B18" s="4" t="inlineStr">
+        <is>
+          <t>Automation Tool Company ATC</t>
+        </is>
+      </c>
+      <c r="C18" s="5" t="inlineStr">
+        <is>
+          <t>Eric Moroge</t>
+        </is>
+      </c>
+      <c r="D18" s="4" t="n">
+        <v>7438426</v>
+      </c>
+      <c r="E18" s="6" t="inlineStr">
+        <is>
+          <t>Trade Show</t>
+        </is>
+      </c>
+      <c r="F18" s="5" t="inlineStr">
+        <is>
+          <t>20251119</t>
+        </is>
+      </c>
+      <c r="G18" s="6" t="n"/>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>ERROR: HTTPConnectionPool(host='localhost', port=58522): Max retries exceeded with url: /session/182bcb18ac3fbf462df686da6b43a0f5/element (Caused by NewConnectionError("HTTPConnection(host='localhost', port=58522): Failed to establish a new connection: [WinError 10061] No connection could be made because the target machine actively refused it"))</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="4" t="n">
+        <v>101034899</v>
+      </c>
+      <c r="B19" s="4" t="inlineStr">
+        <is>
+          <t>Automation Tool Company ATC</t>
+        </is>
+      </c>
+      <c r="C19" s="5" t="inlineStr">
+        <is>
+          <t>Faune Nunnery</t>
+        </is>
+      </c>
+      <c r="D19" s="4" t="n">
+        <v>7438426</v>
+      </c>
+      <c r="E19" s="6" t="inlineStr">
+        <is>
+          <t>Trade Show</t>
+        </is>
+      </c>
+      <c r="F19" s="5" t="inlineStr">
+        <is>
+          <t>20251119</t>
+        </is>
+      </c>
+      <c r="G19" s="6" t="n"/>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>ERROR: HTTPConnectionPool(host='localhost', port=58522): Max retries exceeded with url: /session/182bcb18ac3fbf462df686da6b43a0f5/element (Caused by NewConnectionError("HTTPConnection(host='localhost', port=58522): Failed to establish a new connection: [WinError 10061] No connection could be made because the target machine actively refused it"))</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="4" t="n">
+        <v>101034907</v>
+      </c>
+      <c r="B20" s="4" t="inlineStr">
+        <is>
+          <t>Automation Tool Company ATC</t>
+        </is>
+      </c>
+      <c r="C20" s="5" t="inlineStr">
+        <is>
+          <t>Zeke Shauer</t>
+        </is>
+      </c>
+      <c r="D20" s="4" t="n">
+        <v>7438426</v>
+      </c>
+      <c r="E20" s="6" t="inlineStr">
+        <is>
+          <t>Trade Show</t>
+        </is>
+      </c>
+      <c r="F20" s="5" t="inlineStr">
+        <is>
+          <t>20251119</t>
+        </is>
+      </c>
+      <c r="G20" s="6" t="n"/>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>ERROR: HTTPConnectionPool(host='localhost', port=58522): Max retries exceeded with url: /session/182bcb18ac3fbf462df686da6b43a0f5/element (Caused by NewConnectionError("HTTPConnection(host='localhost', port=58522): Failed to establish a new connection: [WinError 10061] No connection could be made because the target machine actively refused it"))</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="4" t="n">
+        <v>100949915</v>
+      </c>
+      <c r="B21" s="4" t="inlineStr">
+        <is>
+          <t>Automation Tool Company ATC</t>
+        </is>
+      </c>
+      <c r="C21" s="5" t="inlineStr">
+        <is>
+          <t>Phil Walker</t>
+        </is>
+      </c>
+      <c r="D21" s="4" t="n">
+        <v>7438426</v>
+      </c>
+      <c r="E21" s="6" t="inlineStr">
+        <is>
+          <t>Trade Show</t>
+        </is>
+      </c>
+      <c r="F21" s="5" t="inlineStr">
+        <is>
+          <t>20251119</t>
+        </is>
+      </c>
+      <c r="G21" s="6" t="n"/>
+      <c r="H21" t="inlineStr">
+        <is>
           <t xml:space="preserve">ERROR: Message: no such window: target window already closed
 from unknown error: web view not found
   (Session info: chrome=144.0.7559.97)
@@ -576,35 +1222,35 @@
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="4" t="n">
-        <v>120242152</v>
-      </c>
-      <c r="B3" s="4" t="inlineStr">
-        <is>
-          <t>elliTek</t>
-        </is>
-      </c>
-      <c r="C3" s="5" t="inlineStr">
-        <is>
-          <t>alan penticuff</t>
-        </is>
-      </c>
-      <c r="D3" s="4" t="n">
-        <v>120206934</v>
-      </c>
-      <c r="E3" s="6" t="inlineStr">
-        <is>
-          <t>weidmuller cross</t>
-        </is>
-      </c>
-      <c r="F3" s="5" t="inlineStr">
-        <is>
-          <t>20260105</t>
-        </is>
-      </c>
-      <c r="G3" s="6" t="n"/>
-      <c r="H3" t="inlineStr">
+    <row r="22">
+      <c r="A22" s="4" t="n">
+        <v>120053069</v>
+      </c>
+      <c r="B22" s="4" t="inlineStr">
+        <is>
+          <t>Automation Tool Company ATC</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>John Zoodsma</t>
+        </is>
+      </c>
+      <c r="D22" s="4" t="n">
+        <v>7438426</v>
+      </c>
+      <c r="E22" s="6" t="inlineStr">
+        <is>
+          <t>Trade Show</t>
+        </is>
+      </c>
+      <c r="F22" s="5" t="inlineStr">
+        <is>
+          <t>20251119</t>
+        </is>
+      </c>
+      <c r="G22" s="6" t="n"/>
+      <c r="H22" t="inlineStr">
         <is>
           <t xml:space="preserve">ERROR: Message: no such window: target window already closed
 from unknown error: web view not found
@@ -633,35 +1279,35 @@
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="4" t="n">
-        <v>120032621</v>
-      </c>
-      <c r="B4" s="4" t="inlineStr">
-        <is>
-          <t>Control Systems Inc</t>
-        </is>
-      </c>
-      <c r="C4" s="5" t="inlineStr">
-        <is>
-          <t>James Mason</t>
-        </is>
-      </c>
-      <c r="D4" s="4" t="n">
-        <v>120032620</v>
-      </c>
-      <c r="E4" s="6" t="inlineStr">
-        <is>
-          <t>IIAT Visit</t>
-        </is>
-      </c>
-      <c r="F4" s="5" t="inlineStr">
-        <is>
-          <t>20251210</t>
-        </is>
-      </c>
-      <c r="G4" s="6" t="n"/>
-      <c r="H4" t="inlineStr">
+    <row r="23">
+      <c r="A23" s="4" t="n">
+        <v>120293518</v>
+      </c>
+      <c r="B23" s="4" t="inlineStr">
+        <is>
+          <t>Oak Ridge National Laboratory (ORNL)</t>
+        </is>
+      </c>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>Corey Reynolds</t>
+        </is>
+      </c>
+      <c r="D23" s="4" t="n">
+        <v>520170</v>
+      </c>
+      <c r="E23" s="6" t="inlineStr">
+        <is>
+          <t>Teams Meeting</t>
+        </is>
+      </c>
+      <c r="F23" s="5" t="inlineStr">
+        <is>
+          <t>20251120</t>
+        </is>
+      </c>
+      <c r="G23" s="6" t="n"/>
+      <c r="H23" t="inlineStr">
         <is>
           <t xml:space="preserve">ERROR: Message: no such window: target window already closed
 from unknown error: web view not found
@@ -690,35 +1336,35 @@
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="4" t="n">
-        <v>120288152</v>
-      </c>
-      <c r="B5" s="4" t="inlineStr">
-        <is>
-          <t>Control Systems Inc.</t>
-        </is>
-      </c>
-      <c r="C5" s="5" t="inlineStr">
-        <is>
-          <t>Charlie Roberts</t>
-        </is>
-      </c>
-      <c r="D5" s="4" t="n">
-        <v>120032620</v>
-      </c>
-      <c r="E5" s="6" t="inlineStr">
-        <is>
-          <t>IIAT Visit</t>
-        </is>
-      </c>
-      <c r="F5" s="5" t="inlineStr">
-        <is>
-          <t>20251210</t>
-        </is>
-      </c>
-      <c r="G5" s="6" t="n"/>
-      <c r="H5" t="inlineStr">
+    <row r="24">
+      <c r="A24" s="4" t="n">
+        <v>120242173</v>
+      </c>
+      <c r="B24" s="4" t="inlineStr">
+        <is>
+          <t>NRT</t>
+        </is>
+      </c>
+      <c r="C24" s="5" t="inlineStr">
+        <is>
+          <t>drew tooley</t>
+        </is>
+      </c>
+      <c r="D24" s="4" t="n">
+        <v>532951</v>
+      </c>
+      <c r="E24" s="6" t="inlineStr">
+        <is>
+          <t>Lunch HMI Update</t>
+        </is>
+      </c>
+      <c r="F24" s="5" t="inlineStr">
+        <is>
+          <t>20251031</t>
+        </is>
+      </c>
+      <c r="G24" s="6" t="n"/>
+      <c r="H24" t="inlineStr">
         <is>
           <t xml:space="preserve">ERROR: Message: no such window: target window already closed
 from unknown error: web view not found
@@ -747,1089 +1393,6 @@
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="4" t="n">
-        <v>120252514</v>
-      </c>
-      <c r="B6" s="4" t="inlineStr">
-        <is>
-          <t>Rotary Gate Systems</t>
-        </is>
-      </c>
-      <c r="C6" s="5" t="inlineStr">
-        <is>
-          <t>jim knoll</t>
-        </is>
-      </c>
-      <c r="D6" s="4" t="n">
-        <v>120252513</v>
-      </c>
-      <c r="E6" s="6" t="inlineStr">
-        <is>
-          <t>231 application</t>
-        </is>
-      </c>
-      <c r="F6" s="5" t="inlineStr">
-        <is>
-          <t>20251211</t>
-        </is>
-      </c>
-      <c r="G6" s="6" t="n"/>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ERROR: Message: no such window: target window already closed
-from unknown error: web view not found
-  (Session info: chrome=144.0.7559.97)
-Stacktrace:
-Symbols not available. Dumping unresolved backtrace:
-	0x7ff7f391f3d5
-	0x7ff7f391f430
-	0x7ff7f36c10bd
-	0x7ff7f3697c22
-	0x7ff7f374d2a6
-	0x7ff7f3769652
-	0x7ff7f370cb0c
-	0x7ff7f370da53
-	0x7ff7f3bfb470
-	0x7ff7f3bf586d
-	0x7ff7f3c1621a
-	0x7ff7f393b235
-	0x7ff7f3943a5c
-	0x7ff7f3928844
-	0x7ff7f39289f6
-	0x7ff7f390eb87
-	0x7ffde1e7e8d7
-	0x7ffde3bac53c
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="n">
-        <v>120293516</v>
-      </c>
-      <c r="B7" s="4" t="inlineStr">
-        <is>
-          <t>Electric Power Research Institute, Inc EPRI</t>
-        </is>
-      </c>
-      <c r="C7" s="5" t="inlineStr">
-        <is>
-          <t>Ben Ealy</t>
-        </is>
-      </c>
-      <c r="D7" s="4" t="n">
-        <v>120214766</v>
-      </c>
-      <c r="E7" s="6" t="inlineStr">
-        <is>
-          <t>DER Controller Testing</t>
-        </is>
-      </c>
-      <c r="F7" s="5" t="inlineStr">
-        <is>
-          <t>20251105</t>
-        </is>
-      </c>
-      <c r="G7" s="6" t="n"/>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ERROR: Message: no such window: target window already closed
-from unknown error: web view not found
-  (Session info: chrome=144.0.7559.97)
-Stacktrace:
-Symbols not available. Dumping unresolved backtrace:
-	0x7ff7f391f3d5
-	0x7ff7f391f430
-	0x7ff7f36c10bd
-	0x7ff7f3697c22
-	0x7ff7f374d2a6
-	0x7ff7f3769652
-	0x7ff7f370cb0c
-	0x7ff7f370da53
-	0x7ff7f3bfb470
-	0x7ff7f3bf586d
-	0x7ff7f3c1621a
-	0x7ff7f393b235
-	0x7ff7f3943a5c
-	0x7ff7f3928844
-	0x7ff7f39289f6
-	0x7ff7f390eb87
-	0x7ffde1e7e8d7
-	0x7ffde3bac53c
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="4" t="n">
-        <v>120293517</v>
-      </c>
-      <c r="B8" s="4" t="inlineStr">
-        <is>
-          <t>Electric Power Research Institute, Inc EPRI</t>
-        </is>
-      </c>
-      <c r="C8" s="5" t="inlineStr">
-        <is>
-          <t>Ibtissam Kharchouf</t>
-        </is>
-      </c>
-      <c r="D8" s="4" t="n">
-        <v>120214766</v>
-      </c>
-      <c r="E8" s="6" t="inlineStr">
-        <is>
-          <t>DER Controller Testing</t>
-        </is>
-      </c>
-      <c r="F8" s="5" t="inlineStr">
-        <is>
-          <t>20251105</t>
-        </is>
-      </c>
-      <c r="G8" s="6" t="n"/>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ERROR: Message: no such window: target window already closed
-from unknown error: web view not found
-  (Session info: chrome=144.0.7559.97)
-Stacktrace:
-Symbols not available. Dumping unresolved backtrace:
-	0x7ff7f391f3d5
-	0x7ff7f391f430
-	0x7ff7f36c10bd
-	0x7ff7f3697c22
-	0x7ff7f374d2a6
-	0x7ff7f3769652
-	0x7ff7f370cb0c
-	0x7ff7f370da53
-	0x7ff7f3bfb470
-	0x7ff7f3bf586d
-	0x7ff7f3c1621a
-	0x7ff7f393b235
-	0x7ff7f3943a5c
-	0x7ff7f3928844
-	0x7ff7f39289f6
-	0x7ff7f390eb87
-	0x7ffde1e7e8d7
-	0x7ffde3bac53c
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="4" t="n">
-        <v>101035107</v>
-      </c>
-      <c r="B9" s="4" t="inlineStr">
-        <is>
-          <t>Mesa Associates, Inc.</t>
-        </is>
-      </c>
-      <c r="C9" s="5" t="inlineStr">
-        <is>
-          <t>Aneesh Davalbhakta</t>
-        </is>
-      </c>
-      <c r="D9" s="4" t="n">
-        <v>523553</v>
-      </c>
-      <c r="E9" s="6" t="inlineStr">
-        <is>
-          <t>Chris Dunlap meeting - scheduled Lunch n Learn</t>
-        </is>
-      </c>
-      <c r="F9" s="5" t="inlineStr">
-        <is>
-          <t>20251105</t>
-        </is>
-      </c>
-      <c r="G9" s="6" t="n"/>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ERROR: Message: no such window: target window already closed
-from unknown error: web view not found
-  (Session info: chrome=144.0.7559.97)
-Stacktrace:
-Symbols not available. Dumping unresolved backtrace:
-	0x7ff7f391f3d5
-	0x7ff7f391f430
-	0x7ff7f36c10bd
-	0x7ff7f3697c22
-	0x7ff7f374d2a6
-	0x7ff7f3769652
-	0x7ff7f370cb0c
-	0x7ff7f370da53
-	0x7ff7f3bfb470
-	0x7ff7f3bf586d
-	0x7ff7f3c1621a
-	0x7ff7f393b235
-	0x7ff7f3943a5c
-	0x7ff7f3928844
-	0x7ff7f39289f6
-	0x7ff7f390eb87
-	0x7ffde1e7e8d7
-	0x7ffde3bac53c
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="4" t="n">
-        <v>101029218</v>
-      </c>
-      <c r="B10" s="4" t="inlineStr">
-        <is>
-          <t>AUTOMATION NTH</t>
-        </is>
-      </c>
-      <c r="C10" s="5" t="inlineStr">
-        <is>
-          <t>scott weeks</t>
-        </is>
-      </c>
-      <c r="D10" s="4" t="n">
-        <v>522371</v>
-      </c>
-      <c r="E10" s="6" t="inlineStr">
-        <is>
-          <t>Plan lunch n learn</t>
-        </is>
-      </c>
-      <c r="F10" s="5" t="inlineStr">
-        <is>
-          <t>20251106</t>
-        </is>
-      </c>
-      <c r="G10" s="6" t="n"/>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ERROR: Message: no such window: target window already closed
-from unknown error: web view not found
-  (Session info: chrome=144.0.7559.97)
-Stacktrace:
-Symbols not available. Dumping unresolved backtrace:
-	0x7ff7f391f3d5
-	0x7ff7f391f430
-	0x7ff7f36c10bd
-	0x7ff7f3697c22
-	0x7ff7f374d2a6
-	0x7ff7f3769652
-	0x7ff7f370cb0c
-	0x7ff7f370da53
-	0x7ff7f3bfb470
-	0x7ff7f3bf586d
-	0x7ff7f3c1621a
-	0x7ff7f393b235
-	0x7ff7f3943a5c
-	0x7ff7f3928844
-	0x7ff7f39289f6
-	0x7ff7f390eb87
-	0x7ffde1e7e8d7
-	0x7ffde3bac53c
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="4" t="n">
-        <v>100949918</v>
-      </c>
-      <c r="B11" s="4" t="inlineStr">
-        <is>
-          <t>Automation Tool Company ATC</t>
-        </is>
-      </c>
-      <c r="C11" s="5" t="inlineStr">
-        <is>
-          <t>David Bailey</t>
-        </is>
-      </c>
-      <c r="D11" s="4" t="n">
-        <v>7438426</v>
-      </c>
-      <c r="E11" s="6" t="inlineStr">
-        <is>
-          <t>Trade Show</t>
-        </is>
-      </c>
-      <c r="F11" s="5" t="inlineStr">
-        <is>
-          <t>20251119</t>
-        </is>
-      </c>
-      <c r="G11" s="6" t="n"/>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ERROR: Message: no such window: target window already closed
-from unknown error: web view not found
-  (Session info: chrome=144.0.7559.97)
-Stacktrace:
-Symbols not available. Dumping unresolved backtrace:
-	0x7ff7f391f3d5
-	0x7ff7f391f430
-	0x7ff7f36c10bd
-	0x7ff7f3697c22
-	0x7ff7f374d2a6
-	0x7ff7f3769652
-	0x7ff7f370cb0c
-	0x7ff7f370da53
-	0x7ff7f3bfb470
-	0x7ff7f3bf586d
-	0x7ff7f3c1621a
-	0x7ff7f393b235
-	0x7ff7f3943a5c
-	0x7ff7f3928844
-	0x7ff7f39289f6
-	0x7ff7f390eb87
-	0x7ffde1e7e8d7
-	0x7ffde3bac53c
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="4" t="n">
-        <v>100949916</v>
-      </c>
-      <c r="B12" s="4" t="inlineStr">
-        <is>
-          <t>Automation Tool Company ATC</t>
-        </is>
-      </c>
-      <c r="C12" s="5" t="inlineStr">
-        <is>
-          <t>Bobby Buck</t>
-        </is>
-      </c>
-      <c r="D12" s="4" t="n">
-        <v>7438426</v>
-      </c>
-      <c r="E12" s="6" t="inlineStr">
-        <is>
-          <t>Trade Show</t>
-        </is>
-      </c>
-      <c r="F12" s="5" t="inlineStr">
-        <is>
-          <t>20251119</t>
-        </is>
-      </c>
-      <c r="G12" s="6" t="n"/>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ERROR: Message: no such window: target window already closed
-from unknown error: web view not found
-  (Session info: chrome=144.0.7559.97)
-Stacktrace:
-Symbols not available. Dumping unresolved backtrace:
-	0x7ff7f391f3d5
-	0x7ff7f391f430
-	0x7ff7f36c10bd
-	0x7ff7f3697c22
-	0x7ff7f374d2a6
-	0x7ff7f3769652
-	0x7ff7f370cb0c
-	0x7ff7f370da53
-	0x7ff7f3bfb470
-	0x7ff7f3bf586d
-	0x7ff7f3c1621a
-	0x7ff7f393b235
-	0x7ff7f3943a5c
-	0x7ff7f3928844
-	0x7ff7f39289f6
-	0x7ff7f390eb87
-	0x7ffde1e7e8d7
-	0x7ffde3bac53c
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="4" t="n">
-        <v>101092867</v>
-      </c>
-      <c r="B13" s="4" t="inlineStr">
-        <is>
-          <t>Automation Tool Company ATC</t>
-        </is>
-      </c>
-      <c r="C13" s="5" t="inlineStr">
-        <is>
-          <t>Andy Cannon</t>
-        </is>
-      </c>
-      <c r="D13" s="4" t="n">
-        <v>7438426</v>
-      </c>
-      <c r="E13" s="6" t="inlineStr">
-        <is>
-          <t>Trade Show</t>
-        </is>
-      </c>
-      <c r="F13" s="5" t="inlineStr">
-        <is>
-          <t>20251119</t>
-        </is>
-      </c>
-      <c r="G13" s="6" t="n"/>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ERROR: Message: no such window: target window already closed
-from unknown error: web view not found
-  (Session info: chrome=144.0.7559.97)
-Stacktrace:
-Symbols not available. Dumping unresolved backtrace:
-	0x7ff7f391f3d5
-	0x7ff7f391f430
-	0x7ff7f36c10bd
-	0x7ff7f3697c22
-	0x7ff7f374d2a6
-	0x7ff7f3769652
-	0x7ff7f370cb0c
-	0x7ff7f370da53
-	0x7ff7f3bfb470
-	0x7ff7f3bf586d
-	0x7ff7f3c1621a
-	0x7ff7f393b235
-	0x7ff7f3943a5c
-	0x7ff7f3928844
-	0x7ff7f39289f6
-	0x7ff7f390eb87
-	0x7ffde1e7e8d7
-	0x7ffde3bac53c
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="n">
-        <v>101086797</v>
-      </c>
-      <c r="B14" s="4" t="inlineStr">
-        <is>
-          <t>Automation Tool Company ATC</t>
-        </is>
-      </c>
-      <c r="C14" s="5" t="inlineStr">
-        <is>
-          <t>Josh Forgey</t>
-        </is>
-      </c>
-      <c r="D14" s="4" t="n">
-        <v>7438426</v>
-      </c>
-      <c r="E14" s="6" t="inlineStr">
-        <is>
-          <t>Trade Show</t>
-        </is>
-      </c>
-      <c r="F14" s="5" t="inlineStr">
-        <is>
-          <t>20251119</t>
-        </is>
-      </c>
-      <c r="G14" s="6" t="n"/>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ERROR: Message: no such window: target window already closed
-from unknown error: web view not found
-  (Session info: chrome=144.0.7559.97)
-Stacktrace:
-Symbols not available. Dumping unresolved backtrace:
-	0x7ff7f391f3d5
-	0x7ff7f391f430
-	0x7ff7f36c10bd
-	0x7ff7f3697c22
-	0x7ff7f374d2a6
-	0x7ff7f3769652
-	0x7ff7f370cb0c
-	0x7ff7f370da53
-	0x7ff7f3bfb470
-	0x7ff7f3bf586d
-	0x7ff7f3c1621a
-	0x7ff7f393b235
-	0x7ff7f3943a5c
-	0x7ff7f3928844
-	0x7ff7f39289f6
-	0x7ff7f390eb87
-	0x7ffde1e7e8d7
-	0x7ffde3bac53c
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="4" t="n">
-        <v>101140229</v>
-      </c>
-      <c r="B15" s="4" t="inlineStr">
-        <is>
-          <t>Automation Tool Company ATC</t>
-        </is>
-      </c>
-      <c r="C15" s="5" t="inlineStr">
-        <is>
-          <t>Nathan Gooch</t>
-        </is>
-      </c>
-      <c r="D15" s="4" t="n">
-        <v>7438426</v>
-      </c>
-      <c r="E15" s="6" t="inlineStr">
-        <is>
-          <t>Trade Show</t>
-        </is>
-      </c>
-      <c r="F15" s="5" t="inlineStr">
-        <is>
-          <t>20251119</t>
-        </is>
-      </c>
-      <c r="G15" s="6" t="n"/>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ERROR: Message: no such window: target window already closed
-from unknown error: web view not found
-  (Session info: chrome=144.0.7559.97)
-Stacktrace:
-Symbols not available. Dumping unresolved backtrace:
-	0x7ff7f391f3d5
-	0x7ff7f391f430
-	0x7ff7f36c10bd
-	0x7ff7f3697c22
-	0x7ff7f374d2a6
-	0x7ff7f3769652
-	0x7ff7f370cb0c
-	0x7ff7f370da53
-	0x7ff7f3bfb470
-	0x7ff7f3bf586d
-	0x7ff7f3c1621a
-	0x7ff7f393b235
-	0x7ff7f3943a5c
-	0x7ff7f3928844
-	0x7ff7f39289f6
-	0x7ff7f390eb87
-	0x7ffde1e7e8d7
-	0x7ffde3bac53c
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="4" t="n">
-        <v>120053080</v>
-      </c>
-      <c r="B16" s="4" t="inlineStr">
-        <is>
-          <t>Automation Tool Company ATC</t>
-        </is>
-      </c>
-      <c r="C16" s="5" t="inlineStr">
-        <is>
-          <t>Raymond Kilpatrick</t>
-        </is>
-      </c>
-      <c r="D16" s="4" t="n">
-        <v>7438426</v>
-      </c>
-      <c r="E16" s="6" t="inlineStr">
-        <is>
-          <t>Trade Show</t>
-        </is>
-      </c>
-      <c r="F16" s="5" t="inlineStr">
-        <is>
-          <t>20251119</t>
-        </is>
-      </c>
-      <c r="G16" s="6" t="n"/>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ERROR: Message: no such window: target window already closed
-from unknown error: web view not found
-  (Session info: chrome=144.0.7559.97)
-Stacktrace:
-Symbols not available. Dumping unresolved backtrace:
-	0x7ff7f391f3d5
-	0x7ff7f391f430
-	0x7ff7f36c10bd
-	0x7ff7f3697c22
-	0x7ff7f374d2a6
-	0x7ff7f3769652
-	0x7ff7f370cb0c
-	0x7ff7f370da53
-	0x7ff7f3bfb470
-	0x7ff7f3bf586d
-	0x7ff7f3c1621a
-	0x7ff7f393b235
-	0x7ff7f3943a5c
-	0x7ff7f3928844
-	0x7ff7f39289f6
-	0x7ff7f390eb87
-	0x7ffde1e7e8d7
-	0x7ffde3bac53c
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="4" t="n">
-        <v>101035097</v>
-      </c>
-      <c r="B17" s="4" t="inlineStr">
-        <is>
-          <t>Automation Tool Company ATC</t>
-        </is>
-      </c>
-      <c r="C17" s="5" t="inlineStr">
-        <is>
-          <t>Jake McGusland</t>
-        </is>
-      </c>
-      <c r="D17" s="4" t="n">
-        <v>7438426</v>
-      </c>
-      <c r="E17" s="6" t="inlineStr">
-        <is>
-          <t>Trade Show</t>
-        </is>
-      </c>
-      <c r="F17" s="5" t="inlineStr">
-        <is>
-          <t>20251119</t>
-        </is>
-      </c>
-      <c r="G17" s="6" t="n"/>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ERROR: Message: no such window: target window already closed
-from unknown error: web view not found
-  (Session info: chrome=144.0.7559.97)
-Stacktrace:
-Symbols not available. Dumping unresolved backtrace:
-	0x7ff7f391f3d5
-	0x7ff7f391f430
-	0x7ff7f36c10bd
-	0x7ff7f3697c22
-	0x7ff7f374d2a6
-	0x7ff7f3769652
-	0x7ff7f370cb0c
-	0x7ff7f370da53
-	0x7ff7f3bfb470
-	0x7ff7f3bf586d
-	0x7ff7f3c1621a
-	0x7ff7f393b235
-	0x7ff7f3943a5c
-	0x7ff7f3928844
-	0x7ff7f39289f6
-	0x7ff7f390eb87
-	0x7ffde1e7e8d7
-	0x7ffde3bac53c
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="4" t="n">
-        <v>120051335</v>
-      </c>
-      <c r="B18" s="4" t="inlineStr">
-        <is>
-          <t>Automation Tool Company ATC</t>
-        </is>
-      </c>
-      <c r="C18" s="5" t="inlineStr">
-        <is>
-          <t>Eric Moroge</t>
-        </is>
-      </c>
-      <c r="D18" s="4" t="n">
-        <v>7438426</v>
-      </c>
-      <c r="E18" s="6" t="inlineStr">
-        <is>
-          <t>Trade Show</t>
-        </is>
-      </c>
-      <c r="F18" s="5" t="inlineStr">
-        <is>
-          <t>20251119</t>
-        </is>
-      </c>
-      <c r="G18" s="6" t="n"/>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ERROR: Message: no such window: target window already closed
-from unknown error: web view not found
-  (Session info: chrome=144.0.7559.97)
-Stacktrace:
-Symbols not available. Dumping unresolved backtrace:
-	0x7ff7f391f3d5
-	0x7ff7f391f430
-	0x7ff7f36c10bd
-	0x7ff7f3697c22
-	0x7ff7f374d2a6
-	0x7ff7f3769652
-	0x7ff7f370cb0c
-	0x7ff7f370da53
-	0x7ff7f3bfb470
-	0x7ff7f3bf586d
-	0x7ff7f3c1621a
-	0x7ff7f393b235
-	0x7ff7f3943a5c
-	0x7ff7f3928844
-	0x7ff7f39289f6
-	0x7ff7f390eb87
-	0x7ffde1e7e8d7
-	0x7ffde3bac53c
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="4" t="n">
-        <v>101034899</v>
-      </c>
-      <c r="B19" s="4" t="inlineStr">
-        <is>
-          <t>Automation Tool Company ATC</t>
-        </is>
-      </c>
-      <c r="C19" s="5" t="inlineStr">
-        <is>
-          <t>Faune Nunnery</t>
-        </is>
-      </c>
-      <c r="D19" s="4" t="n">
-        <v>7438426</v>
-      </c>
-      <c r="E19" s="6" t="inlineStr">
-        <is>
-          <t>Trade Show</t>
-        </is>
-      </c>
-      <c r="F19" s="5" t="inlineStr">
-        <is>
-          <t>20251119</t>
-        </is>
-      </c>
-      <c r="G19" s="6" t="n"/>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ERROR: Message: no such window: target window already closed
-from unknown error: web view not found
-  (Session info: chrome=144.0.7559.97)
-Stacktrace:
-Symbols not available. Dumping unresolved backtrace:
-	0x7ff7f391f3d5
-	0x7ff7f391f430
-	0x7ff7f36c10bd
-	0x7ff7f3697c22
-	0x7ff7f374d2a6
-	0x7ff7f3769652
-	0x7ff7f370cb0c
-	0x7ff7f370da53
-	0x7ff7f3bfb470
-	0x7ff7f3bf586d
-	0x7ff7f3c1621a
-	0x7ff7f393b235
-	0x7ff7f3943a5c
-	0x7ff7f3928844
-	0x7ff7f39289f6
-	0x7ff7f390eb87
-	0x7ffde1e7e8d7
-	0x7ffde3bac53c
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="4" t="n">
-        <v>101034907</v>
-      </c>
-      <c r="B20" s="4" t="inlineStr">
-        <is>
-          <t>Automation Tool Company ATC</t>
-        </is>
-      </c>
-      <c r="C20" s="5" t="inlineStr">
-        <is>
-          <t>Zeke Shauer</t>
-        </is>
-      </c>
-      <c r="D20" s="4" t="n">
-        <v>7438426</v>
-      </c>
-      <c r="E20" s="6" t="inlineStr">
-        <is>
-          <t>Trade Show</t>
-        </is>
-      </c>
-      <c r="F20" s="5" t="inlineStr">
-        <is>
-          <t>20251119</t>
-        </is>
-      </c>
-      <c r="G20" s="6" t="n"/>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ERROR: Message: no such window: target window already closed
-from unknown error: web view not found
-  (Session info: chrome=144.0.7559.97)
-Stacktrace:
-Symbols not available. Dumping unresolved backtrace:
-	0x7ff7f391f3d5
-	0x7ff7f391f430
-	0x7ff7f36c10bd
-	0x7ff7f3697c22
-	0x7ff7f374d2a6
-	0x7ff7f3769652
-	0x7ff7f370cb0c
-	0x7ff7f370da53
-	0x7ff7f3bfb470
-	0x7ff7f3bf586d
-	0x7ff7f3c1621a
-	0x7ff7f393b235
-	0x7ff7f3943a5c
-	0x7ff7f3928844
-	0x7ff7f39289f6
-	0x7ff7f390eb87
-	0x7ffde1e7e8d7
-	0x7ffde3bac53c
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="4" t="n">
-        <v>100949915</v>
-      </c>
-      <c r="B21" s="4" t="inlineStr">
-        <is>
-          <t>Automation Tool Company ATC</t>
-        </is>
-      </c>
-      <c r="C21" s="5" t="inlineStr">
-        <is>
-          <t>Phil Walker</t>
-        </is>
-      </c>
-      <c r="D21" s="4" t="n">
-        <v>7438426</v>
-      </c>
-      <c r="E21" s="6" t="inlineStr">
-        <is>
-          <t>Trade Show</t>
-        </is>
-      </c>
-      <c r="F21" s="5" t="inlineStr">
-        <is>
-          <t>20251119</t>
-        </is>
-      </c>
-      <c r="G21" s="6" t="n"/>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ERROR: Message: no such window: target window already closed
-from unknown error: web view not found
-  (Session info: chrome=144.0.7559.97)
-Stacktrace:
-Symbols not available. Dumping unresolved backtrace:
-	0x7ff7f391f3d5
-	0x7ff7f391f430
-	0x7ff7f36c10bd
-	0x7ff7f3697c22
-	0x7ff7f374d2a6
-	0x7ff7f3769652
-	0x7ff7f370cb0c
-	0x7ff7f370da53
-	0x7ff7f3bfb470
-	0x7ff7f3bf586d
-	0x7ff7f3c1621a
-	0x7ff7f393b235
-	0x7ff7f3943a5c
-	0x7ff7f3928844
-	0x7ff7f39289f6
-	0x7ff7f390eb87
-	0x7ffde1e7e8d7
-	0x7ffde3bac53c
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="4" t="n">
-        <v>120053069</v>
-      </c>
-      <c r="B22" s="4" t="inlineStr">
-        <is>
-          <t>Automation Tool Company ATC</t>
-        </is>
-      </c>
-      <c r="C22" s="5" t="inlineStr">
-        <is>
-          <t>John Zoodsma</t>
-        </is>
-      </c>
-      <c r="D22" s="4" t="n">
-        <v>7438426</v>
-      </c>
-      <c r="E22" s="6" t="inlineStr">
-        <is>
-          <t>Trade Show</t>
-        </is>
-      </c>
-      <c r="F22" s="5" t="inlineStr">
-        <is>
-          <t>20251119</t>
-        </is>
-      </c>
-      <c r="G22" s="6" t="n"/>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ERROR: Message: no such window: target window already closed
-from unknown error: web view not found
-  (Session info: chrome=144.0.7559.97)
-Stacktrace:
-Symbols not available. Dumping unresolved backtrace:
-	0x7ff7f391f3d5
-	0x7ff7f391f430
-	0x7ff7f36c10bd
-	0x7ff7f3697c22
-	0x7ff7f374d2a6
-	0x7ff7f3769652
-	0x7ff7f370cb0c
-	0x7ff7f370da53
-	0x7ff7f3bfb470
-	0x7ff7f3bf586d
-	0x7ff7f3c1621a
-	0x7ff7f393b235
-	0x7ff7f3943a5c
-	0x7ff7f3928844
-	0x7ff7f39289f6
-	0x7ff7f390eb87
-	0x7ffde1e7e8d7
-	0x7ffde3bac53c
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="4" t="n">
-        <v>120293518</v>
-      </c>
-      <c r="B23" s="4" t="inlineStr">
-        <is>
-          <t>Oak Ridge National Laboratory (ORNL)</t>
-        </is>
-      </c>
-      <c r="C23" s="5" t="inlineStr">
-        <is>
-          <t>Corey Reynolds</t>
-        </is>
-      </c>
-      <c r="D23" s="4" t="n">
-        <v>520170</v>
-      </c>
-      <c r="E23" s="6" t="inlineStr">
-        <is>
-          <t>Teams Meeting</t>
-        </is>
-      </c>
-      <c r="F23" s="5" t="inlineStr">
-        <is>
-          <t>20251120</t>
-        </is>
-      </c>
-      <c r="G23" s="6" t="n"/>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ERROR: Message: no such window: target window already closed
-from unknown error: web view not found
-  (Session info: chrome=144.0.7559.97)
-Stacktrace:
-Symbols not available. Dumping unresolved backtrace:
-	0x7ff7f391f3d5
-	0x7ff7f391f430
-	0x7ff7f36c10bd
-	0x7ff7f3697c22
-	0x7ff7f374d2a6
-	0x7ff7f3769652
-	0x7ff7f370cb0c
-	0x7ff7f370da53
-	0x7ff7f3bfb470
-	0x7ff7f3bf586d
-	0x7ff7f3c1621a
-	0x7ff7f393b235
-	0x7ff7f3943a5c
-	0x7ff7f3928844
-	0x7ff7f39289f6
-	0x7ff7f390eb87
-	0x7ffde1e7e8d7
-	0x7ffde3bac53c
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="4" t="n">
-        <v>120242173</v>
-      </c>
-      <c r="B24" s="4" t="inlineStr">
-        <is>
-          <t>NRT</t>
-        </is>
-      </c>
-      <c r="C24" s="5" t="inlineStr">
-        <is>
-          <t>drew tooley</t>
-        </is>
-      </c>
-      <c r="D24" s="4" t="n">
-        <v>532951</v>
-      </c>
-      <c r="E24" s="6" t="inlineStr">
-        <is>
-          <t>Lunch HMI Update</t>
-        </is>
-      </c>
-      <c r="F24" s="5" t="inlineStr">
-        <is>
-          <t>20251031</t>
-        </is>
-      </c>
-      <c r="G24" s="6" t="n"/>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ERROR: Message: no such window: target window already closed
-from unknown error: web view not found
-  (Session info: chrome=144.0.7559.97)
-Stacktrace:
-Symbols not available. Dumping unresolved backtrace:
-	0x7ff7f391f3d5
-	0x7ff7f391f430
-	0x7ff7f36c10bd
-	0x7ff7f3697c22
-	0x7ff7f374d2a6
-	0x7ff7f3769652
-	0x7ff7f370cb0c
-	0x7ff7f370da53
-	0x7ff7f3bfb470
-	0x7ff7f3bf586d
-	0x7ff7f3c1621a
-	0x7ff7f393b235
-	0x7ff7f3943a5c
-	0x7ff7f3928844
-	0x7ff7f39289f6
-	0x7ff7f390eb87
-	0x7ffde1e7e8d7
-	0x7ffde3bac53c
-</t>
-        </is>
-      </c>
-    </row>
     <row r="25">
       <c r="A25" s="4" t="n"/>
       <c r="B25" s="4" t="n"/>

</xml_diff>

<commit_message>
add adv excel sheet
</commit_message>
<xml_diff>
--- a/Log Activity.xlsx
+++ b/Log Activity.xlsx
@@ -1195,30 +1195,7 @@
       <c r="G21" s="6" t="n"/>
       <c r="H21" t="inlineStr">
         <is>
-          <t xml:space="preserve">ERROR: Message: no such window: target window already closed
-from unknown error: web view not found
-  (Session info: chrome=144.0.7559.97)
-Stacktrace:
-Symbols not available. Dumping unresolved backtrace:
-	0x7ff7f391f3d5
-	0x7ff7f391f430
-	0x7ff7f36c10bd
-	0x7ff7f3697c22
-	0x7ff7f374d2a6
-	0x7ff7f3769652
-	0x7ff7f370cb0c
-	0x7ff7f370da53
-	0x7ff7f3bfb470
-	0x7ff7f3bf586d
-	0x7ff7f3c1621a
-	0x7ff7f393b235
-	0x7ff7f3943a5c
-	0x7ff7f3928844
-	0x7ff7f39289f6
-	0x7ff7f390eb87
-	0x7ffde1e7e8d7
-	0x7ffde3bac53c
-</t>
+          <t>ERROR: HTTPConnectionPool(host='localhost', port=58522): Max retries exceeded with url: /session/182bcb18ac3fbf462df686da6b43a0f5/element (Caused by NewConnectionError("HTTPConnection(host='localhost', port=58522): Failed to establish a new connection: [WinError 10061] No connection could be made because the target machine actively refused it"))</t>
         </is>
       </c>
     </row>
@@ -1252,30 +1229,7 @@
       <c r="G22" s="6" t="n"/>
       <c r="H22" t="inlineStr">
         <is>
-          <t xml:space="preserve">ERROR: Message: no such window: target window already closed
-from unknown error: web view not found
-  (Session info: chrome=144.0.7559.97)
-Stacktrace:
-Symbols not available. Dumping unresolved backtrace:
-	0x7ff7f391f3d5
-	0x7ff7f391f430
-	0x7ff7f36c10bd
-	0x7ff7f3697c22
-	0x7ff7f374d2a6
-	0x7ff7f3769652
-	0x7ff7f370cb0c
-	0x7ff7f370da53
-	0x7ff7f3bfb470
-	0x7ff7f3bf586d
-	0x7ff7f3c1621a
-	0x7ff7f393b235
-	0x7ff7f3943a5c
-	0x7ff7f3928844
-	0x7ff7f39289f6
-	0x7ff7f390eb87
-	0x7ffde1e7e8d7
-	0x7ffde3bac53c
-</t>
+          <t>ERROR: HTTPConnectionPool(host='localhost', port=58522): Max retries exceeded with url: /session/182bcb18ac3fbf462df686da6b43a0f5/element (Caused by NewConnectionError("HTTPConnection(host='localhost', port=58522): Failed to establish a new connection: [WinError 10061] No connection could be made because the target machine actively refused it"))</t>
         </is>
       </c>
     </row>
@@ -1309,30 +1263,7 @@
       <c r="G23" s="6" t="n"/>
       <c r="H23" t="inlineStr">
         <is>
-          <t xml:space="preserve">ERROR: Message: no such window: target window already closed
-from unknown error: web view not found
-  (Session info: chrome=144.0.7559.97)
-Stacktrace:
-Symbols not available. Dumping unresolved backtrace:
-	0x7ff7f391f3d5
-	0x7ff7f391f430
-	0x7ff7f36c10bd
-	0x7ff7f3697c22
-	0x7ff7f374d2a6
-	0x7ff7f3769652
-	0x7ff7f370cb0c
-	0x7ff7f370da53
-	0x7ff7f3bfb470
-	0x7ff7f3bf586d
-	0x7ff7f3c1621a
-	0x7ff7f393b235
-	0x7ff7f3943a5c
-	0x7ff7f3928844
-	0x7ff7f39289f6
-	0x7ff7f390eb87
-	0x7ffde1e7e8d7
-	0x7ffde3bac53c
-</t>
+          <t>ERROR: HTTPConnectionPool(host='localhost', port=58522): Max retries exceeded with url: /session/182bcb18ac3fbf462df686da6b43a0f5/element (Caused by NewConnectionError("HTTPConnection(host='localhost', port=58522): Failed to establish a new connection: [WinError 10061] No connection could be made because the target machine actively refused it"))</t>
         </is>
       </c>
     </row>
@@ -1366,30 +1297,7 @@
       <c r="G24" s="6" t="n"/>
       <c r="H24" t="inlineStr">
         <is>
-          <t xml:space="preserve">ERROR: Message: no such window: target window already closed
-from unknown error: web view not found
-  (Session info: chrome=144.0.7559.97)
-Stacktrace:
-Symbols not available. Dumping unresolved backtrace:
-	0x7ff7f391f3d5
-	0x7ff7f391f430
-	0x7ff7f36c10bd
-	0x7ff7f3697c22
-	0x7ff7f374d2a6
-	0x7ff7f3769652
-	0x7ff7f370cb0c
-	0x7ff7f370da53
-	0x7ff7f3bfb470
-	0x7ff7f3bf586d
-	0x7ff7f3c1621a
-	0x7ff7f393b235
-	0x7ff7f3943a5c
-	0x7ff7f3928844
-	0x7ff7f39289f6
-	0x7ff7f390eb87
-	0x7ffde1e7e8d7
-	0x7ffde3bac53c
-</t>
+          <t>ERROR: HTTPConnectionPool(host='localhost', port=58522): Max retries exceeded with url: /session/182bcb18ac3fbf462df686da6b43a0f5/element (Caused by NewConnectionError("HTTPConnection(host='localhost', port=58522): Failed to establish a new connection: [WinError 10061] No connection could be made because the target machine actively refused it"))</t>
         </is>
       </c>
     </row>

</xml_diff>